<commit_message>
add materials for sessions 2-4
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/GitHub/24-2-ia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF2422E-74E0-4249-A73F-57522AB72BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C32A751-5C64-8742-B213-8C00B987B343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="920" windowWidth="29100" windowHeight="16820" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -135,6 +135,18 @@
   </si>
   <si>
     <t>prep/p02.html</t>
+  </si>
+  <si>
+    <t>exercises/e03.html</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-03-eine-problemstellung-entwickeln</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-02-parasoziale-beziehungen-im-zeitverlauf</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-04-grundlagen-der-manuellen-inhaltsanalyse</t>
   </si>
 </sst>
 </file>
@@ -490,7 +502,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -554,6 +566,9 @@
       <c r="D3" t="s">
         <v>32</v>
       </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
       <c r="G3" t="s">
         <v>19</v>
       </c>
@@ -568,6 +583,12 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
       <c r="G4" t="s">
         <v>20</v>
       </c>
@@ -581,6 +602,9 @@
       </c>
       <c r="C5" t="s">
         <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
add task for session 04
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/GitHub/24-2-ia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C32A751-5C64-8742-B213-8C00B987B343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ABC24F-A8A0-4144-976F-093D13D13B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="920" windowWidth="29100" windowHeight="16820" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -137,9 +137,6 @@
     <t>prep/p02.html</t>
   </si>
   <si>
-    <t>exercises/e03.html</t>
-  </si>
-  <si>
     <t>slides/slides.html#/sitzung-03-eine-problemstellung-entwickeln</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>slides/slides.html#/sitzung-04-grundlagen-der-manuellen-inhaltsanalyse</t>
+  </si>
+  <si>
+    <t>exercises/e04.html</t>
   </si>
 </sst>
 </file>
@@ -502,7 +502,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,7 +567,7 @@
         <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
@@ -584,9 +584,6 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" t="s">
         <v>33</v>
       </c>
       <c r="G4" t="s">
@@ -604,6 +601,9 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
         <v>36</v>
       </c>
       <c r="G5" t="s">

</xml_diff>

<commit_message>
add materials for session 05
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/GitHub/24-2-ia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12ABC24F-A8A0-4144-976F-093D13D13B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0838B9B4-71FD-3847-99D7-55DE3875190C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="920" windowWidth="29100" windowHeight="16820" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -128,25 +128,31 @@
     <t>Aufgaben</t>
   </si>
   <si>
+    <t>Automatisierte Inhaltsanalyse 2: Zero-Shot Klassifikation</t>
+  </si>
+  <si>
+    <t>prep/p02.html</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-03-eine-problemstellung-entwickeln</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-02-parasoziale-beziehungen-im-zeitverlauf</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-04-grundlagen-der-manuellen-inhaltsanalyse</t>
+  </si>
+  <si>
+    <t>exercises/e04.html</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-05-chancen-risiken-automatisierter-methoden</t>
+  </si>
+  <si>
+    <t>https://stats.ifp.uni-mainz.de/ba-ccs-track/ia-daten.html</t>
+  </si>
+  <si>
     <t>Automatisierte Inhaltsanalyse 1: Datenerhebung</t>
-  </si>
-  <si>
-    <t>Automatisierte Inhaltsanalyse 2: Zero-Shot Klassifikation</t>
-  </si>
-  <si>
-    <t>prep/p02.html</t>
-  </si>
-  <si>
-    <t>slides/slides.html#/sitzung-03-eine-problemstellung-entwickeln</t>
-  </si>
-  <si>
-    <t>slides/slides.html#/sitzung-02-parasoziale-beziehungen-im-zeitverlauf</t>
-  </si>
-  <si>
-    <t>slides/slides.html#/sitzung-04-grundlagen-der-manuellen-inhaltsanalyse</t>
-  </si>
-  <si>
-    <t>exercises/e04.html</t>
   </si>
 </sst>
 </file>
@@ -502,7 +508,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -564,10 +570,10 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
@@ -584,7 +590,7 @@
         <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
         <v>20</v>
@@ -601,10 +607,10 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
         <v>35</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
       </c>
       <c r="G5" t="s">
         <v>17</v>
@@ -620,6 +626,9 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
       <c r="G6" t="s">
         <v>19</v>
       </c>
@@ -632,7 +641,10 @@
         <v>45624</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
       </c>
       <c r="G7" t="s">
         <v>17</v>
@@ -646,7 +658,7 @@
         <v>45631</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
add exercise for session 06
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/GitHub/24-2-ia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0838B9B4-71FD-3847-99D7-55DE3875190C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED931F9-D14D-DB4B-84A5-E38E1244701F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="920" windowWidth="29100" windowHeight="16820" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>Automatisierte Inhaltsanalyse 1: Datenerhebung</t>
+  </si>
+  <si>
+    <t>exercises/e06.html</t>
+  </si>
+  <si>
+    <t>https://stats.ifp.uni-mainz.de/ba-ccs-track/ia-zeroshot.html</t>
   </si>
 </sst>
 </file>
@@ -508,7 +514,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,6 +652,9 @@
       <c r="D7" t="s">
         <v>37</v>
       </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
       <c r="G7" t="s">
         <v>17</v>
       </c>
@@ -659,6 +668,9 @@
       </c>
       <c r="C8" t="s">
         <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>40</v>
       </c>
       <c r="G8" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
add slides for session 06
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/GitHub/24-2-ia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED931F9-D14D-DB4B-84A5-E38E1244701F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525855E6-CCC7-8F40-9206-978B2946E4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="920" windowWidth="29100" windowHeight="16820" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>https://stats.ifp.uni-mainz.de/ba-ccs-track/ia-zeroshot.html</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-06-automatisierte-inhaltsanalyse-1-datenerhebung</t>
   </si>
 </sst>
 </file>
@@ -514,7 +517,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -652,6 +655,9 @@
       <c r="D7" t="s">
         <v>37</v>
       </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
       <c r="F7" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
add materials for session 07
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/GitHub/24-2-ia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525855E6-CCC7-8F40-9206-978B2946E4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBFFC14-4B1C-BB4E-ACF6-123E0079F0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="920" windowWidth="29100" windowHeight="16820" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -162,6 +162,12 @@
   </si>
   <si>
     <t>slides/slides.html#/sitzung-06-automatisierte-inhaltsanalyse-1-datenerhebung</t>
+  </si>
+  <si>
+    <t>exercises/e07.html</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-07-automatisierte-inhaltsanalyse-1-zero-shot-klassifikation</t>
   </si>
 </sst>
 </file>
@@ -517,7 +523,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,6 +684,12 @@
       <c r="D8" t="s">
         <v>40</v>
       </c>
+      <c r="E8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
       <c r="G8" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
add material for session 09
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/GitHub/24-2-ia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5B6A03-BE13-8341-9E3B-7F8B15C39B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC8918E-40D4-354C-A71A-5D2709101100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="920" windowWidth="29100" windowHeight="16820" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>slides/slides.html#/sitzung-08-codebuch-goldstandard</t>
+  </si>
+  <si>
+    <t>exercises/e09.html</t>
   </si>
 </sst>
 </file>
@@ -529,7 +532,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,6 +733,9 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
+      <c r="F10" t="s">
+        <v>46</v>
+      </c>
       <c r="G10" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
add info materials for reliability tests / session 10
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/GitHub/24-2-ia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC8918E-40D4-354C-A71A-5D2709101100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20A4507-BBD6-4C4C-BAA6-F8D77260F9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="920" windowWidth="29100" windowHeight="16820" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>exercises/e09.html</t>
+  </si>
+  <si>
+    <t>https://stats.ifp.uni-mainz.de/ba-ccs-track/ia-reli-vali.html</t>
   </si>
 </sst>
 </file>
@@ -532,7 +535,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -759,6 +762,9 @@
       <c r="C12" t="s">
         <v>24</v>
       </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
       <c r="G12" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
add exercise for session 10
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/GitHub/24-2-ia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20A4507-BBD6-4C4C-BAA6-F8D77260F9FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357C4EF8-533E-0E46-82CE-16DA0FB2E6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="920" windowWidth="29100" windowHeight="16820" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>https://stats.ifp.uni-mainz.de/ba-ccs-track/ia-reli-vali.html</t>
+  </si>
+  <si>
+    <t>exercises/e10.html</t>
   </si>
 </sst>
 </file>
@@ -535,7 +538,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -765,6 +768,9 @@
       <c r="D12" t="s">
         <v>47</v>
       </c>
+      <c r="F12" t="s">
+        <v>48</v>
+      </c>
       <c r="G12" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
add materials for final session
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/GitHub/24-2-ia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D95E7B-DA83-D841-AF45-4ACF3B4C574D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784663AF-07E9-BA44-A373-7FF3E0313413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="920" windowWidth="29100" windowHeight="16820" xr2:uid="{8F9E752D-D0F4-2F4B-82F2-3A0B3F0631FE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
   <si>
     <t>exercises/e01.html</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>slides/slides.html#/sitzung-11-hypothesentests</t>
+  </si>
+  <si>
+    <t>slides/slides.html#/sitzung-14-semesterabschluss-und-informationen-zum-projektbericht</t>
   </si>
 </sst>
 </file>
@@ -541,7 +544,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -833,6 +836,9 @@
       <c r="C16" t="s">
         <v>11</v>
       </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
       <c r="G16" t="s">
         <v>17</v>
       </c>

</xml_diff>